<commit_message>
adding automatic nucleus determination
</commit_message>
<xml_diff>
--- a/paper2/glm/predictorSettings.xlsx
+++ b/paper2/glm/predictorSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\github\locomotionAnalysis\paper2\glm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214510E3-9986-4E80-9048-42556A3CBAEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444D21B6-070F-4205-8C95-21358FF15184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5715" windowWidth="28800" windowHeight="15885" activeTab="1" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
+    <workbookView xWindow="9600" yWindow="5715" windowWidth="28800" windowHeight="15885" activeTab="1" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
   </bookViews>
   <sheets>
     <sheet name="predictors" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,30 @@
     <author>Richard Warren</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{B0AFD67C-9992-48F5-8A75-31400D4766EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Richard Warren:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+space separated list of predictor groups to be 'explained away' before building models using this group // use to determine how much unique deviance is explained bythe predictor group</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{BD4FA76A-1DF2-48CA-84D4-6AA08633DFA7}">
       <text>
         <r>
@@ -96,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -373,6 +397,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1225,7 +1253,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,6 +1298,9 @@
       <c r="A4" t="s">
         <v>43</v>
       </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
adding epoch models, trained in certain periods and tested in other periods
</commit_message>
<xml_diff>
--- a/paper2/glm/predictorSettings.xlsx
+++ b/paper2/glm/predictorSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\github\locomotionAnalysis\paper2\glm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C14EBD-75CC-4454-B856-1F50A857B797}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB0587-4199-434D-990E-49A030775AD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-195" yWindow="-60" windowWidth="2400" windowHeight="585" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="7500" windowHeight="6000" xr2:uid="{4669D966-A741-4C3C-B919-B304607B653B}"/>
   </bookViews>
   <sheets>
     <sheet name="predictors" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>name</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>response</t>
+  </si>
+  <si>
+    <t>lickRate</t>
   </si>
 </sst>
 </file>
@@ -696,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E69B2E9-D98C-4615-9F0D-8BE0A12B27A9}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,6 +1238,17 @@
         <v>1</v>
       </c>
       <c r="H41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>